<commit_message>
Got heartbeat functionality working
</commit_message>
<xml_diff>
--- a/hdw/KiCad_Project/Electronic_Calendar/Electronic_Calendar.xlsx
+++ b/hdw/KiCad_Project/Electronic_Calendar/Electronic_Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic-Calendar\hdw\KiCad_Project\Electronic_Calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D7FB2A0F-908A-4DB2-A934-A9888349D316}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BF1157-2D13-440B-BB26-D829E2D59752}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020"/>
+    <workbookView xWindow="38280" yWindow="3540" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronic_Calendar" sheetId="1" r:id="rId1"/>
@@ -526,92 +526,92 @@
     <t>296-26275-1-ND</t>
   </si>
   <si>
+    <t>C301, C302</t>
+  </si>
+  <si>
+    <t>C308, C310</t>
+  </si>
+  <si>
+    <t>C1508, C1509</t>
+  </si>
+  <si>
+    <t>D1001, D1003, D1006, D1101</t>
+  </si>
+  <si>
+    <t>D1005, D1102, D1103, D1104, D1105, D1106, D1201, D1202, D1203, D1204, D1205, D1206, D1207, D1208, D1209, D1210, D1211, D1212, D1213, D1214, D1215, D1216, D1217, D1218, D1219, D1220, D1221, D1222, D1223, D1224, D1225, D1226, D1227, D1228, D1229, D1230, D1231, D1232, D1233, D1234, D1235, D1236, D1237, D1238, D1239, D1240, D1241, D1242, D1243, D1244, D1245, D1246, D1247, D1248, D1249, D1250, D1251, D1252, D1253, D1254, D1255, D1256, D1257, D1258, D1301, D1302, D1303, D1304, D1305, D1306, D1307, D1308, D1309, D1310, D1311, D1312, D1313, D1314, D1315, D1316, D1317, D1318, D1319, D1320, D1321</t>
+  </si>
+  <si>
+    <t>L801, L802, L1501, L1502</t>
+  </si>
+  <si>
+    <t>Q201, Q202</t>
+  </si>
+  <si>
+    <t>R203, R401, R402, R407</t>
+  </si>
+  <si>
+    <t>R204, R302, R307, R310</t>
+  </si>
+  <si>
+    <t>R209, R309</t>
+  </si>
+  <si>
+    <t>R303, R308</t>
+  </si>
+  <si>
+    <t>R404, R405, R901, R1703, R1704, R1705, R1711, R1712</t>
+  </si>
+  <si>
+    <t>R606, R1001, R1003, R1005, R1006, R1103, R1104, R1107, R1108, R1111, R1112, R1201, R1202, R1203, R1204, R1301, R1302, R1303, R1304, R1305, R1306, R1307, R1308, R1309, R1310, R1311, R1312, R1313, R1314, R1315, R1316, R1317, R1318, R1319, R1320, R1321, R1510</t>
+  </si>
+  <si>
+    <t>R1508, R1509</t>
+  </si>
+  <si>
+    <t>U202, U302</t>
+  </si>
+  <si>
+    <t>U402, U801</t>
+  </si>
+  <si>
+    <t>U1001, U1003, U1006, U1101, U1102, U1103, U1104, U1105, U1106</t>
+  </si>
+  <si>
+    <t>U1401, U1402, U1403, U1404, U1405</t>
+  </si>
+  <si>
+    <t>U1601, U1602, U1603, U1604</t>
+  </si>
+  <si>
+    <t>U1701, U1702, U1703, U1705, U1706</t>
+  </si>
+  <si>
+    <t>D301, D1601, D1602</t>
+  </si>
+  <si>
+    <t>C203, C207, C208, C314, C317, C805, C806, C811, C812, C817, C818, C823, C824, C904, C1607, C1608, C1609, C1612, C1705, C1706, C1713, C1721, C1722</t>
+  </si>
+  <si>
+    <t>C312, C315, C402, C403, C404</t>
+  </si>
+  <si>
+    <t>C202, C206, C304, C313, C803, C804, C809, C810, C815, C816, C821, C822, C901, C903, C1604, C1605, C1606, C1611, C1703, C1704, C1707, C1708, C1711, C1715, C1719, C1720, C1723, C1724</t>
+  </si>
+  <si>
     <t>C201, C204, C205, C305, C307, C311, C316, C401, C601, C602, C801, C802, C807, C808, C813, C814, C819, C820, C825, C902, C1001, C1003, C1005, C1006, C1101, C1102, C1103, C1104, C1105, C1106, C1401, C1402, C1403, C1404, C1405, C1501, C1502, C1503, C1504, C1506, C1507, C1510, C1601, C1602, C1603, C1610, C1701, C1702, C1709, C1717, C1718</t>
   </si>
   <si>
-    <t>C202, C206, C304, C313, C803, C804, C809, C810, C815, C816, C821, C822, C901, C903, C1604, C1605, C1606, C1611, C1703, C1704, C1707, C1708, C1711, C1715, C1719, C1720, C1723, C1724</t>
-  </si>
-  <si>
-    <t>C203, C207, C208, C314, C317, C805, C806, C811, C812, C817, C818, C823, C824, C904, C1607, C1608, C1609, C1612, C1705, C1706, C1713, C1721, C1722</t>
-  </si>
-  <si>
-    <t>C301, C302</t>
-  </si>
-  <si>
-    <t>C308, C310</t>
-  </si>
-  <si>
-    <t>C312, C315, C402, C403, C404</t>
-  </si>
-  <si>
-    <t>C1508, C1509</t>
-  </si>
-  <si>
-    <t>D301, D1601, D1602</t>
-  </si>
-  <si>
-    <t>D1001, D1003, D1006, D1101</t>
-  </si>
-  <si>
-    <t>D1005, D1102, D1103, D1104, D1105, D1106, D1201, D1202, D1203, D1204, D1205, D1206, D1207, D1208, D1209, D1210, D1211, D1212, D1213, D1214, D1215, D1216, D1217, D1218, D1219, D1220, D1221, D1222, D1223, D1224, D1225, D1226, D1227, D1228, D1229, D1230, D1231, D1232, D1233, D1234, D1235, D1236, D1237, D1238, D1239, D1240, D1241, D1242, D1243, D1244, D1245, D1246, D1247, D1248, D1249, D1250, D1251, D1252, D1253, D1254, D1255, D1256, D1257, D1258, D1301, D1302, D1303, D1304, D1305, D1306, D1307, D1308, D1309, D1310, D1311, D1312, D1313, D1314, D1315, D1316, D1317, D1318, D1319, D1320, D1321</t>
-  </si>
-  <si>
-    <t>L801, L802, L1501, L1502</t>
-  </si>
-  <si>
-    <t>Q201, Q202</t>
-  </si>
-  <si>
-    <t>R203, R401, R402, R407</t>
-  </si>
-  <si>
-    <t>R204, R302, R307, R310</t>
-  </si>
-  <si>
     <t>R205, R206, R304, R601</t>
   </si>
   <si>
     <t>R207, R301, R403, R406, R602, R604, R801, R902, R1101, R1102, R1105, R1106, R1109, R1110, R1401, R1402, R1403, R1404, R1405, R1406, R1407, R1408, R1409, R1410, R1411, R1412, R1413, R1414, R1415, R1416, R1417, R1418, R1419, R1420, R1421, R1422, R1423, R1424, R1501, R1505, R1506, R1507, R1607, R1608, R1609, R1610, R1611, R1612, R1615, R1616, R1701, R1702, R1707, R1709, R1710</t>
-  </si>
-  <si>
-    <t>R209, R309</t>
-  </si>
-  <si>
-    <t>R303, R308</t>
-  </si>
-  <si>
-    <t>R404, R405, R901, R1703, R1704, R1705, R1711, R1712</t>
-  </si>
-  <si>
-    <t>R606, R1001, R1003, R1005, R1006, R1103, R1104, R1107, R1108, R1111, R1112, R1201, R1202, R1203, R1204, R1301, R1302, R1303, R1304, R1305, R1306, R1307, R1308, R1309, R1310, R1311, R1312, R1313, R1314, R1315, R1316, R1317, R1318, R1319, R1320, R1321, R1510</t>
-  </si>
-  <si>
-    <t>R1508, R1509</t>
-  </si>
-  <si>
-    <t>U202, U302</t>
-  </si>
-  <si>
-    <t>U402, U801</t>
-  </si>
-  <si>
-    <t>U1001, U1003, U1006, U1101, U1102, U1103, U1104, U1105, U1106</t>
-  </si>
-  <si>
-    <t>U1401, U1402, U1403, U1404, U1405</t>
-  </si>
-  <si>
-    <t>U1601, U1602, U1603, U1604</t>
-  </si>
-  <si>
-    <t>U1701, U1702, U1703, U1705, U1706</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,6 +742,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1088,9 +1095,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1447,11 +1457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,8 +1503,8 @@
       <c r="A3" s="1">
         <v>51</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>168</v>
+      <c r="B3" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1507,8 +1517,8 @@
       <c r="A4" s="1">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>169</v>
+      <c r="B4" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1521,8 +1531,8 @@
       <c r="A5" s="1">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>170</v>
+      <c r="B5" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -1535,7 +1545,7 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1549,8 +1559,8 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>171</v>
+      <c r="B7" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -1563,7 +1573,7 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1577,8 +1587,8 @@
       <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>172</v>
+      <c r="B9" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
@@ -1591,7 +1601,7 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1605,8 +1615,8 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>173</v>
+      <c r="B11" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>26</v>
@@ -1619,7 +1629,7 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1633,8 +1643,8 @@
       <c r="A13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>174</v>
+      <c r="B13" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>31</v>
@@ -1647,7 +1657,7 @@
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1661,8 +1671,8 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>175</v>
+      <c r="B15" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -1675,8 +1685,8 @@
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>176</v>
+      <c r="B16" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -1689,8 +1699,8 @@
       <c r="A17" s="1">
         <v>85</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>177</v>
+      <c r="B17" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>40</v>
@@ -1703,7 +1713,7 @@
       <c r="A18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1777,7 +1787,7 @@
       <c r="A24" s="1">
         <v>1</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1791,7 +1801,7 @@
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1805,7 +1815,7 @@
       <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1819,7 +1829,7 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1833,8 +1843,8 @@
       <c r="A28" s="1">
         <v>4</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>178</v>
+      <c r="B28" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>67</v>
@@ -1847,8 +1857,8 @@
       <c r="A29" s="1">
         <v>2</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>179</v>
+      <c r="B29" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>69</v>
@@ -1861,7 +1871,7 @@
       <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1873,7 +1883,7 @@
       <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1887,7 +1897,7 @@
       <c r="A32" s="1">
         <v>1</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1901,7 +1911,7 @@
       <c r="A33" s="1">
         <v>1</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1915,8 +1925,8 @@
       <c r="A34" s="1">
         <v>4</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>180</v>
+      <c r="B34" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>82</v>
@@ -1929,8 +1939,8 @@
       <c r="A35" s="1">
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>181</v>
+      <c r="B35" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>84</v>
@@ -1943,8 +1953,8 @@
       <c r="A36" s="1">
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>182</v>
+      <c r="B36" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="C36" s="1">
         <v>10</v>
@@ -1957,8 +1967,8 @@
       <c r="A37" s="1">
         <v>55</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>183</v>
+      <c r="B37" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>87</v>
@@ -1971,7 +1981,7 @@
       <c r="A38" s="1">
         <v>1</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1985,8 +1995,8 @@
       <c r="A39" s="1">
         <v>2</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>184</v>
+      <c r="B39" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="C39" s="1">
         <v>0.02</v>
@@ -1999,7 +2009,7 @@
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -2013,8 +2023,8 @@
       <c r="A41" s="1">
         <v>2</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>185</v>
+      <c r="B41" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>96</v>
@@ -2027,7 +2037,7 @@
       <c r="A42" s="1">
         <v>1</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -2041,7 +2051,7 @@
       <c r="A43" s="1">
         <v>1</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2055,8 +2065,8 @@
       <c r="A44" s="1">
         <v>8</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>186</v>
+      <c r="B44" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="C44" s="1">
         <v>499</v>
@@ -2069,7 +2079,7 @@
       <c r="A45" s="1">
         <v>1</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C45" s="1">
@@ -2083,7 +2093,7 @@
       <c r="A46" s="1">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="1">
@@ -2097,8 +2107,8 @@
       <c r="A47" s="1">
         <v>37</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>187</v>
+      <c r="B47" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>109</v>
@@ -2111,7 +2121,7 @@
       <c r="A48" s="1">
         <v>1</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2125,7 +2135,7 @@
       <c r="A49" s="1">
         <v>1</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2139,7 +2149,7 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2153,8 +2163,8 @@
       <c r="A51" s="1">
         <v>2</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>188</v>
+      <c r="B51" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="C51" s="1">
         <v>27</v>
@@ -2167,7 +2177,7 @@
       <c r="A52" s="1">
         <v>1</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2181,7 +2191,7 @@
       <c r="A53" s="1">
         <v>1</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -2195,7 +2205,7 @@
       <c r="A54" s="1">
         <v>1</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2207,7 +2217,7 @@
       <c r="A55" s="1">
         <v>1</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2221,8 +2231,8 @@
       <c r="A56" s="1">
         <v>2</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>189</v>
+      <c r="B56" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>132</v>
@@ -2235,7 +2245,7 @@
       <c r="A57" s="1">
         <v>1</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2249,7 +2259,7 @@
       <c r="A58" s="1">
         <v>1</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2263,8 +2273,8 @@
       <c r="A59" s="1">
         <v>2</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>190</v>
+      <c r="B59" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>140</v>
@@ -2277,7 +2287,7 @@
       <c r="A60" s="1">
         <v>1</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2291,7 +2301,7 @@
       <c r="A61" s="1">
         <v>1</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -2305,8 +2315,8 @@
       <c r="A62" s="1">
         <v>9</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>191</v>
+      <c r="B62" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>148</v>
@@ -2319,7 +2329,7 @@
       <c r="A63" s="1">
         <v>1</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2333,8 +2343,8 @@
       <c r="A64" s="1">
         <v>5</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>192</v>
+      <c r="B64" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>153</v>
@@ -2347,7 +2357,7 @@
       <c r="A65" s="1">
         <v>1</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -2361,7 +2371,7 @@
       <c r="A66" s="1">
         <v>1</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -2375,7 +2385,7 @@
       <c r="A67" s="1">
         <v>1</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2389,8 +2399,8 @@
       <c r="A68" s="1">
         <v>4</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>193</v>
+      <c r="B68" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>164</v>
@@ -2403,8 +2413,8 @@
       <c r="A69" s="1">
         <v>5</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>194</v>
+      <c r="B69" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>166</v>
@@ -2415,5 +2425,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>